<commit_message>
almost finished disease burden comparison
</commit_message>
<xml_diff>
--- a/Shiny_app/Disease_burden.xlsx
+++ b/Shiny_app/Disease_burden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/Shiny_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC7D258-7F5B-6D44-BAAA-6F17A7ECDC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0C06C0-473C-7549-87C7-E4882BC68F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{8779009B-6560-994C-AF4D-251485407F43}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="165">
   <si>
     <t>Therapeutic_Area</t>
   </si>
@@ -906,6 +906,15 @@
   </si>
   <si>
     <t>2014-2018</t>
+  </si>
+  <si>
+    <t>Indication</t>
+  </si>
+  <si>
+    <t>Burden_Metric</t>
+  </si>
+  <si>
+    <t>Burden_Year</t>
   </si>
 </sst>
 </file>
@@ -1378,26 +1387,16 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1422,16 +1421,26 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1755,8 +1764,8 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1779,13 +1788,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>59</v>
@@ -1913,19 +1922,19 @@
       <c r="D16">
         <v>2019</v>
       </c>
-      <c r="E16" s="81">
+      <c r="E16" s="58">
         <f>'Hep-C'!N24</f>
         <v>1.1490754128300739E-2</v>
       </c>
-      <c r="F16" s="81">
+      <c r="F16" s="58">
         <f>'Hep-C'!N25</f>
         <v>0.14559013773685411</v>
       </c>
-      <c r="G16" s="81">
+      <c r="G16" s="58">
         <f>'Hep-C'!N27</f>
         <v>5.9554067422570578E-2</v>
       </c>
-      <c r="H16" s="81">
+      <c r="H16" s="58">
         <f>'Hep-C'!N26</f>
         <v>0.7581462597975801</v>
       </c>
@@ -1937,10 +1946,10 @@
       <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="81"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1949,10 +1958,10 @@
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="81"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1967,19 +1976,19 @@
       <c r="D19">
         <v>2018</v>
       </c>
-      <c r="E19" s="81">
+      <c r="E19" s="58">
         <f>'HIV-1'!D6</f>
         <v>0.02</v>
       </c>
-      <c r="F19" s="81">
+      <c r="F19" s="58">
         <f>'HIV-1'!D5</f>
         <v>0.42</v>
       </c>
-      <c r="G19" s="81">
+      <c r="G19" s="58">
         <f>'HIV-1'!D4</f>
         <v>0.27</v>
       </c>
-      <c r="H19" s="81">
+      <c r="H19" s="58">
         <f>'HIV-1'!D9</f>
         <v>0.28331015592077546</v>
       </c>
@@ -1988,10 +1997,10 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -2000,10 +2009,10 @@
       <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -2012,10 +2021,10 @@
       <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -2024,10 +2033,10 @@
       <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2036,10 +2045,10 @@
       <c r="B24" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -2048,10 +2057,10 @@
       <c r="B25" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -2060,10 +2069,10 @@
       <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="81"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -2078,19 +2087,19 @@
       <c r="D27" t="s">
         <v>161</v>
       </c>
-      <c r="E27" s="81">
+      <c r="E27" s="58">
         <f>Oncology!F16</f>
         <v>4.2589254369253961E-2</v>
       </c>
-      <c r="F27" s="81">
+      <c r="F27" s="58">
         <f>Oncology!F17</f>
         <v>0.11372597555393253</v>
       </c>
-      <c r="G27" s="81">
+      <c r="G27" s="58">
         <f>Oncology!F18</f>
         <v>0.14203150432043035</v>
       </c>
-      <c r="H27" s="81">
+      <c r="H27" s="58">
         <f>Oncology!F19</f>
         <v>0.68841815470559131</v>
       </c>
@@ -2102,10 +2111,10 @@
       <c r="B28" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -2120,19 +2129,19 @@
       <c r="D29" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="81">
+      <c r="E29" s="58">
         <f>Oncology!F24</f>
         <v>4.9130655205846162E-2</v>
       </c>
-      <c r="F29" s="81">
+      <c r="F29" s="58">
         <f>Oncology!F25</f>
         <v>0.14710906220566675</v>
       </c>
-      <c r="G29" s="81">
+      <c r="G29" s="58">
         <f>Oncology!F26</f>
         <v>9.7848954647604874E-2</v>
       </c>
-      <c r="H29" s="81">
+      <c r="H29" s="58">
         <f>Oncology!F27</f>
         <v>0.69105617632588867</v>
       </c>
@@ -2150,19 +2159,19 @@
       <c r="D30" t="s">
         <v>161</v>
       </c>
-      <c r="E30" s="81">
+      <c r="E30" s="58">
         <f>Oncology!F32</f>
         <v>4.4629723165078052E-3</v>
       </c>
-      <c r="F30" s="81">
+      <c r="F30" s="58">
         <f>Oncology!F33</f>
         <v>6.1504111859382359E-3</v>
       </c>
-      <c r="G30" s="81">
+      <c r="G30" s="58">
         <f>Oncology!F34</f>
         <v>4.1819875738818658E-2</v>
       </c>
-      <c r="H30" s="81">
+      <c r="H30" s="58">
         <f>Oncology!F35</f>
         <v>0.94216050564711784</v>
       </c>
@@ -2180,19 +2189,19 @@
       <c r="D31" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="81">
+      <c r="E31" s="58">
         <f>Oncology!F40</f>
         <v>3.4130643808144512E-2</v>
       </c>
-      <c r="F31" s="81">
+      <c r="F31" s="58">
         <f>Oncology!F41</f>
         <v>8.7787587767109279E-2</v>
       </c>
-      <c r="G31" s="81">
+      <c r="G31" s="58">
         <f>Oncology!F42</f>
         <v>0.10487041252137158</v>
       </c>
-      <c r="H31" s="81">
+      <c r="H31" s="58">
         <f>Oncology!F43</f>
         <v>0.76245086838236054</v>
       </c>
@@ -2210,19 +2219,19 @@
       <c r="D32" t="s">
         <v>161</v>
       </c>
-      <c r="E32" s="81">
+      <c r="E32" s="58">
         <f>Oncology!F48</f>
         <v>5.0646412840369588E-2</v>
       </c>
-      <c r="F32" s="81">
+      <c r="F32" s="58">
         <f>Oncology!F49</f>
         <v>0.10897024280854647</v>
       </c>
-      <c r="G32" s="81">
+      <c r="G32" s="58">
         <f>Oncology!F50</f>
         <v>0.16756919165727702</v>
       </c>
-      <c r="H32" s="81">
+      <c r="H32" s="58">
         <f>Oncology!F51</f>
         <v>0.66129859603298036</v>
       </c>
@@ -2240,19 +2249,19 @@
       <c r="D33" t="s">
         <v>161</v>
       </c>
-      <c r="E33" s="81">
+      <c r="E33" s="58">
         <f>Oncology!F56</f>
         <v>3.6934969321592605E-2</v>
       </c>
-      <c r="F33" s="81">
+      <c r="F33" s="58">
         <f>Oncology!F57</f>
         <v>0.2240070060967943</v>
       </c>
-      <c r="G33" s="81">
+      <c r="G33" s="58">
         <f>Oncology!F58</f>
         <v>0.14465439394012025</v>
       </c>
-      <c r="H33" s="81">
+      <c r="H33" s="58">
         <f>Oncology!F59</f>
         <v>0.58467150181376448</v>
       </c>
@@ -2270,19 +2279,19 @@
       <c r="D34" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="81">
+      <c r="E34" s="58">
         <f>Oncology!F8</f>
         <v>3.6376828768558259E-2</v>
       </c>
-      <c r="F34" s="81">
+      <c r="F34" s="58">
         <f>Oncology!F9</f>
         <v>0.262966924406141</v>
       </c>
-      <c r="G34" s="81">
+      <c r="G34" s="58">
         <f>Oncology!F10</f>
         <v>0.16420869409121366</v>
       </c>
-      <c r="H34" s="81">
+      <c r="H34" s="58">
         <f>Oncology!F11</f>
         <v>0.52055035297817032</v>
       </c>
@@ -2300,19 +2309,19 @@
       <c r="D35" t="s">
         <v>161</v>
       </c>
-      <c r="E35" s="81">
+      <c r="E35" s="58">
         <f>Oncology!F64</f>
         <v>5.9676119856498365E-2</v>
       </c>
-      <c r="F35" s="81">
+      <c r="F35" s="58">
         <f>Oncology!F65</f>
         <v>0.14149798543558961</v>
       </c>
-      <c r="G35" s="81">
+      <c r="G35" s="58">
         <f>Oncology!F66</f>
         <v>0.13529195744728761</v>
       </c>
-      <c r="H35" s="81">
+      <c r="H35" s="58">
         <f>Oncology!F67</f>
         <v>0.65065578411486813</v>
       </c>
@@ -4471,62 +4480,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="2.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
     </row>
     <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
     </row>
     <row r="3" spans="1:20" s="27" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="75">
+      <c r="B3" s="67">
         <v>40269</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="77" t="s">
+      <c r="C3" s="68"/>
+      <c r="D3" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
     </row>
     <row r="4" spans="1:20" s="29" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="74"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="28" t="s">
         <v>112</v>
       </c>
@@ -9440,120 +9449,120 @@
       </c>
     </row>
     <row r="131" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="78" t="s">
+      <c r="A131" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="B131" s="79"/>
-      <c r="C131" s="79"/>
-      <c r="D131" s="79"/>
-      <c r="E131" s="79"/>
-      <c r="F131" s="79"/>
-      <c r="G131" s="79"/>
-      <c r="H131" s="79"/>
-      <c r="I131" s="79"/>
-      <c r="J131" s="79"/>
-      <c r="K131" s="79"/>
-      <c r="L131" s="79"/>
-      <c r="M131" s="80"/>
+      <c r="B131" s="60"/>
+      <c r="C131" s="60"/>
+      <c r="D131" s="60"/>
+      <c r="E131" s="60"/>
+      <c r="F131" s="60"/>
+      <c r="G131" s="60"/>
+      <c r="H131" s="60"/>
+      <c r="I131" s="60"/>
+      <c r="J131" s="60"/>
+      <c r="K131" s="60"/>
+      <c r="L131" s="60"/>
+      <c r="M131" s="61"/>
     </row>
     <row r="132" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="58" t="s">
+      <c r="A132" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="B132" s="59"/>
-      <c r="C132" s="59"/>
-      <c r="D132" s="59"/>
-      <c r="E132" s="59"/>
-      <c r="F132" s="59"/>
-      <c r="G132" s="59"/>
-      <c r="H132" s="59"/>
-      <c r="I132" s="59"/>
-      <c r="J132" s="59"/>
-      <c r="K132" s="59"/>
-      <c r="L132" s="59"/>
-      <c r="M132" s="60"/>
+      <c r="B132" s="71"/>
+      <c r="C132" s="71"/>
+      <c r="D132" s="71"/>
+      <c r="E132" s="71"/>
+      <c r="F132" s="71"/>
+      <c r="G132" s="71"/>
+      <c r="H132" s="71"/>
+      <c r="I132" s="71"/>
+      <c r="J132" s="71"/>
+      <c r="K132" s="71"/>
+      <c r="L132" s="71"/>
+      <c r="M132" s="72"/>
     </row>
     <row r="133" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="61" t="s">
+      <c r="A133" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="B133" s="62"/>
-      <c r="C133" s="62"/>
-      <c r="D133" s="62"/>
-      <c r="E133" s="62"/>
-      <c r="F133" s="62"/>
-      <c r="G133" s="62"/>
-      <c r="H133" s="62"/>
-      <c r="I133" s="62"/>
-      <c r="J133" s="62"/>
-      <c r="K133" s="62"/>
-      <c r="L133" s="62"/>
-      <c r="M133" s="63"/>
+      <c r="B133" s="74"/>
+      <c r="C133" s="74"/>
+      <c r="D133" s="74"/>
+      <c r="E133" s="74"/>
+      <c r="F133" s="74"/>
+      <c r="G133" s="74"/>
+      <c r="H133" s="74"/>
+      <c r="I133" s="74"/>
+      <c r="J133" s="74"/>
+      <c r="K133" s="74"/>
+      <c r="L133" s="74"/>
+      <c r="M133" s="75"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="64" t="s">
+      <c r="A134" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="B134" s="65"/>
-      <c r="C134" s="65"/>
-      <c r="D134" s="65"/>
-      <c r="E134" s="65"/>
-      <c r="F134" s="65"/>
-      <c r="G134" s="65"/>
-      <c r="H134" s="65"/>
-      <c r="I134" s="65"/>
-      <c r="J134" s="65"/>
-      <c r="K134" s="65"/>
-      <c r="L134" s="65"/>
-      <c r="M134" s="66"/>
+      <c r="B134" s="77"/>
+      <c r="C134" s="77"/>
+      <c r="D134" s="77"/>
+      <c r="E134" s="77"/>
+      <c r="F134" s="77"/>
+      <c r="G134" s="77"/>
+      <c r="H134" s="77"/>
+      <c r="I134" s="77"/>
+      <c r="J134" s="77"/>
+      <c r="K134" s="77"/>
+      <c r="L134" s="77"/>
+      <c r="M134" s="78"/>
     </row>
     <row r="135" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="64" t="s">
+      <c r="A135" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="B135" s="65"/>
-      <c r="C135" s="65"/>
-      <c r="D135" s="65"/>
-      <c r="E135" s="65"/>
-      <c r="F135" s="65"/>
-      <c r="G135" s="65"/>
-      <c r="H135" s="65"/>
-      <c r="I135" s="65"/>
-      <c r="J135" s="65"/>
-      <c r="K135" s="65"/>
-      <c r="L135" s="65"/>
-      <c r="M135" s="66"/>
+      <c r="B135" s="77"/>
+      <c r="C135" s="77"/>
+      <c r="D135" s="77"/>
+      <c r="E135" s="77"/>
+      <c r="F135" s="77"/>
+      <c r="G135" s="77"/>
+      <c r="H135" s="77"/>
+      <c r="I135" s="77"/>
+      <c r="J135" s="77"/>
+      <c r="K135" s="77"/>
+      <c r="L135" s="77"/>
+      <c r="M135" s="78"/>
     </row>
     <row r="136" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="67" t="s">
+      <c r="A136" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="B136" s="68"/>
-      <c r="C136" s="68"/>
-      <c r="D136" s="68"/>
-      <c r="E136" s="68"/>
-      <c r="F136" s="68"/>
-      <c r="G136" s="68"/>
-      <c r="H136" s="68"/>
-      <c r="I136" s="68"/>
-      <c r="J136" s="68"/>
-      <c r="K136" s="68"/>
-      <c r="L136" s="68"/>
-      <c r="M136" s="69"/>
+      <c r="B136" s="80"/>
+      <c r="C136" s="80"/>
+      <c r="D136" s="80"/>
+      <c r="E136" s="80"/>
+      <c r="F136" s="80"/>
+      <c r="G136" s="80"/>
+      <c r="H136" s="80"/>
+      <c r="I136" s="80"/>
+      <c r="J136" s="80"/>
+      <c r="K136" s="80"/>
+      <c r="L136" s="80"/>
+      <c r="M136" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A132:M132"/>
+    <mergeCell ref="A133:M133"/>
+    <mergeCell ref="A134:M134"/>
+    <mergeCell ref="A135:M135"/>
+    <mergeCell ref="A136:M136"/>
     <mergeCell ref="A131:M131"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:M3"/>
-    <mergeCell ref="A132:M132"/>
-    <mergeCell ref="A133:M133"/>
-    <mergeCell ref="A134:M134"/>
-    <mergeCell ref="A135:M135"/>
-    <mergeCell ref="A136:M136"/>
   </mergeCells>
   <pageMargins left="0.25" right="0" top="0.75" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToWidth="2" fitToHeight="6" orientation="landscape" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
shared this version w others
</commit_message>
<xml_diff>
--- a/Shiny_app/Disease_burden.xlsx
+++ b/Shiny_app/Disease_burden.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/Shiny_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0C06C0-473C-7549-87C7-E4882BC68F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA96E80-9CE2-F042-AF1A-86C5566CB212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{8779009B-6560-994C-AF4D-251485407F43}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{8779009B-6560-994C-AF4D-251485407F43}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -1764,8 +1764,8 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>